<commit_message>
Added Extent Report support, added Listener classes
</commit_message>
<xml_diff>
--- a/src/test/resources/LoginData.xlsx
+++ b/src/test/resources/LoginData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="16095" windowHeight="3030"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16755" windowHeight="2145"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
@@ -12,70 +12,47 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <si>
+    <t>testme1@gmail.com</t>
+  </si>
   <si>
     <t>pass123</t>
   </si>
   <si>
+    <t>testme2@gmail.com</t>
+  </si>
+  <si>
     <t>pass124</t>
   </si>
   <si>
+    <t>testme3@gmail.com</t>
+  </si>
+  <si>
     <t>pass125</t>
   </si>
   <si>
+    <t>testme4@gmail.com</t>
+  </si>
+  <si>
+    <t>pass126</t>
+  </si>
+  <si>
+    <t>testme5@gmail.com</t>
+  </si>
+  <si>
+    <t>pass127</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
     <t>Password</t>
-  </si>
-  <si>
-    <t>Mail_Id</t>
-  </si>
-  <si>
-    <t>TATestme1@gmail.com</t>
-  </si>
-  <si>
-    <t>TATestme2@gmail.com</t>
-  </si>
-  <si>
-    <t>TATestme3@gmail.com</t>
-  </si>
-  <si>
-    <t>TATestme4@gmail.com</t>
-  </si>
-  <si>
-    <t>pass126</t>
-  </si>
-  <si>
-    <t>TATestme5@gmail.com</t>
-  </si>
-  <si>
-    <t>pass127</t>
-  </si>
-  <si>
-    <t>TATestme6@gmail.com</t>
-  </si>
-  <si>
-    <t>pass128</t>
-  </si>
-  <si>
-    <t>TATestme7@gmail.com</t>
-  </si>
-  <si>
-    <t>pass129</t>
-  </si>
-  <si>
-    <t>TATestme8@gmail.com</t>
-  </si>
-  <si>
-    <t>pass130</t>
-  </si>
-  <si>
-    <t>TATestme9@gmail.com</t>
-  </si>
-  <si>
-    <t>pass131</t>
   </si>
 </sst>
 </file>
@@ -431,87 +408,74 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
-      </c>
+      <c r="A7" s="1"/>
     </row>
     <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
+      <c r="A8" s="1"/>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
+      <c r="A9" s="1"/>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
+      <c r="A10" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="A5" r:id="rId3"/>
+    <hyperlink ref="A4" r:id="rId4"/>
+    <hyperlink ref="A6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>